<commit_message>
Update of Traceability Matrix Template test and design Test_Plan.xls  template  created
</commit_message>
<xml_diff>
--- a/WL Project/V-Cycle Process/V_Cycle Process Script.xlsx
+++ b/WL Project/V-Cycle Process/V_Cycle Process Script.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\myRepository Github\trunk\WL Project\V-Cycle Process\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7890" yWindow="3180" windowWidth="15015" windowHeight="9330" activeTab="3"/>
+    <workbookView xWindow="7890" yWindow="3180" windowWidth="15015" windowHeight="9330"/>
   </bookViews>
   <sheets>
     <sheet name="V-Cycle" sheetId="2" r:id="rId1"/>
@@ -1990,9 +1990,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Hoja1"/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
@@ -2004,10 +2005,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Hoja2"/>
   <dimension ref="C2:E33"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2229,6 +2231,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Hoja3"/>
   <dimension ref="C2:E27"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -2406,9 +2409,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Hoja4"/>
   <dimension ref="C2:E31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -2620,6 +2624,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Hoja5"/>
   <dimension ref="C2:E25"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
@@ -2785,6 +2790,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Hoja6"/>
   <dimension ref="C2:E32"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">

</xml_diff>

<commit_message>
modified the dummy.c an error indexing 5 in an incorrect place but cppcheck prevent me update links from Traceability Matrix Template.xls and revise the design specifications document DSD_template.doc
</commit_message>
<xml_diff>
--- a/WL Project/V-Cycle Process/V_Cycle Process Script.xlsx
+++ b/WL Project/V-Cycle Process/V_Cycle Process Script.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7890" yWindow="3180" windowWidth="15015" windowHeight="9330" activeTab="3"/>
+    <workbookView xWindow="7890" yWindow="3180" windowWidth="15015" windowHeight="9330" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="V-Cycle" sheetId="2" r:id="rId1"/>
@@ -2008,8 +2008,8 @@
   <sheetPr codeName="Hoja2"/>
   <dimension ref="C2:E33"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2412,7 +2412,7 @@
   <sheetPr codeName="Hoja4"/>
   <dimension ref="C2:E31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>

</xml_diff>